<commit_message>
removing ablation study from git
</commit_message>
<xml_diff>
--- a/sidewalk-vs-street/Ablation-study-diary.xlsx
+++ b/sidewalk-vs-street/Ablation-study-diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beatr\Desktop\UIUC classes\CS498 ML in Wireless Systems\micromobility-iot-ml\sidewalk-vs-street\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1996D7-B9AD-4453-AD29-346FD5A54D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDF99D9-68A5-48B7-8924-FC4E88008B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10440" xr2:uid="{6A800C74-5ABE-4F2B-885A-C955F89BD598}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Ablation study diary</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Window size 150</t>
+  </si>
+  <si>
+    <t>street_classifier_2021_12_03_12_30_57</t>
+  </si>
+  <si>
+    <t>Window size 50, rbf in SVC classifier</t>
   </si>
 </sst>
 </file>
@@ -406,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{739F5443-5482-4E8D-8C83-77FD71872365}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,6 +452,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>